<commit_message>
Fixed codes for registers vs. immediate
</commit_message>
<xml_diff>
--- a/Docs/MachineCode.xlsx
+++ b/Docs/MachineCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4780" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MachineCode" sheetId="2" r:id="rId1"/>
@@ -650,8 +650,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -779,7 +789,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -822,6 +832,11 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -864,6 +879,11 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1196,7 +1216,7 @@
   <dimension ref="A1:AI78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AG78"/>
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6543,8 +6563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:AO78"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62:AO63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6593,14 +6613,14 @@
       <c r="M2" s="11">
         <v>1</v>
       </c>
-      <c r="N2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>112</v>
+      <c r="N2" s="11">
+        <v>0</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2" s="11">
+        <v>0</v>
       </c>
       <c r="Q2" s="11" t="s">
         <v>112</v>
@@ -6609,13 +6629,13 @@
         <v>112</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V2" s="11" t="s">
         <v>113</v>
@@ -6623,14 +6643,14 @@
       <c r="W2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X2" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="11">
-        <v>0</v>
+      <c r="X2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AA2" s="11">
         <v>0</v>
@@ -6712,14 +6732,14 @@
       <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="N3" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>112</v>
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
+        <v>1</v>
       </c>
       <c r="Q3" s="14" t="s">
         <v>112</v>
@@ -6727,14 +6747,14 @@
       <c r="R3" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S3" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>113</v>
+      <c r="S3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" t="s">
+        <v>112</v>
+      </c>
+      <c r="U3" t="s">
+        <v>112</v>
       </c>
       <c r="V3" s="14" t="s">
         <v>113</v>
@@ -6775,14 +6795,14 @@
       <c r="AH3" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AI3" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="14">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="14">
-        <v>0</v>
+      <c r="AI3" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ3" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK3" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AL3" s="14">
         <v>0</v>
@@ -7057,14 +7077,14 @@
       <c r="M8" s="11">
         <v>0</v>
       </c>
-      <c r="N8" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>112</v>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>112</v>
@@ -7073,13 +7093,13 @@
         <v>112</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V8" s="11" t="s">
         <v>113</v>
@@ -7087,14 +7107,14 @@
       <c r="W8" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X8" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="11">
-        <v>0</v>
+      <c r="X8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AA8" s="11">
         <v>0</v>
@@ -7167,14 +7187,14 @@
       <c r="M9" s="14">
         <v>0</v>
       </c>
-      <c r="N9" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>112</v>
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <v>1</v>
       </c>
       <c r="Q9" s="14" t="s">
         <v>112</v>
@@ -7182,14 +7202,14 @@
       <c r="R9" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S9" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="U9" s="14" t="s">
-        <v>113</v>
+      <c r="S9" t="s">
+        <v>112</v>
+      </c>
+      <c r="T9" t="s">
+        <v>112</v>
+      </c>
+      <c r="U9" t="s">
+        <v>112</v>
       </c>
       <c r="V9" s="14" t="s">
         <v>113</v>
@@ -7230,14 +7250,14 @@
       <c r="AH9" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AI9" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="14">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="14">
-        <v>0</v>
+      <c r="AI9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK9" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AL9" s="14">
         <v>0</v>
@@ -7521,14 +7541,14 @@
       <c r="M14" s="11">
         <v>0</v>
       </c>
-      <c r="N14" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P14" s="11" t="s">
-        <v>112</v>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11">
+        <v>0</v>
+      </c>
+      <c r="P14" s="11">
+        <v>0</v>
       </c>
       <c r="Q14" s="11" t="s">
         <v>112</v>
@@ -7537,13 +7557,13 @@
         <v>112</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V14" s="11" t="s">
         <v>113</v>
@@ -7551,14 +7571,14 @@
       <c r="W14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X14" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="11">
-        <v>0</v>
+      <c r="X14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AA14" s="11">
         <v>0</v>
@@ -7631,14 +7651,14 @@
       <c r="M15" s="14">
         <v>0</v>
       </c>
-      <c r="N15" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P15" s="14" t="s">
-        <v>112</v>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="14">
+        <v>0</v>
+      </c>
+      <c r="P15" s="14">
+        <v>1</v>
       </c>
       <c r="Q15" s="14" t="s">
         <v>112</v>
@@ -7646,14 +7666,14 @@
       <c r="R15" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S15" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="T15" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="U15" s="14" t="s">
-        <v>113</v>
+      <c r="S15" t="s">
+        <v>112</v>
+      </c>
+      <c r="T15" t="s">
+        <v>112</v>
+      </c>
+      <c r="U15" t="s">
+        <v>112</v>
       </c>
       <c r="V15" s="14" t="s">
         <v>113</v>
@@ -7694,14 +7714,14 @@
       <c r="AH15" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AI15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="14">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="14">
-        <v>0</v>
+      <c r="AI15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK15" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AL15" s="14">
         <v>0</v>
@@ -10547,14 +10567,14 @@
       <c r="M50" s="11">
         <v>0</v>
       </c>
-      <c r="N50" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="O50" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P50" s="11" t="s">
-        <v>112</v>
+      <c r="N50" s="11">
+        <v>0</v>
+      </c>
+      <c r="O50" s="11">
+        <v>0</v>
+      </c>
+      <c r="P50" s="11">
+        <v>0</v>
       </c>
       <c r="Q50" s="11" t="s">
         <v>112</v>
@@ -10563,13 +10583,13 @@
         <v>112</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T50" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V50" s="11" t="s">
         <v>113</v>
@@ -10577,14 +10597,14 @@
       <c r="W50" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X50" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="11">
-        <v>0</v>
+      <c r="X50" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y50" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z50" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AA50" s="11">
         <v>0</v>
@@ -10660,14 +10680,14 @@
       <c r="M51" s="14">
         <v>0</v>
       </c>
-      <c r="N51" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O51" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P51" s="14" t="s">
-        <v>112</v>
+      <c r="N51" s="14">
+        <v>0</v>
+      </c>
+      <c r="O51" s="14">
+        <v>0</v>
+      </c>
+      <c r="P51" s="14">
+        <v>1</v>
       </c>
       <c r="Q51" s="14" t="s">
         <v>112</v>
@@ -10675,14 +10695,14 @@
       <c r="R51" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S51" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="T51" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="U51" s="14" t="s">
-        <v>113</v>
+      <c r="S51" t="s">
+        <v>112</v>
+      </c>
+      <c r="T51" t="s">
+        <v>112</v>
+      </c>
+      <c r="U51" t="s">
+        <v>112</v>
       </c>
       <c r="V51" s="14" t="s">
         <v>113</v>
@@ -10723,14 +10743,14 @@
       <c r="AH51" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AI51" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ51" s="14">
-        <v>0</v>
-      </c>
-      <c r="AK51" s="14">
-        <v>0</v>
+      <c r="AI51" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ51" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK51" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AL51" s="14">
         <v>0</v>
@@ -11006,14 +11026,14 @@
       <c r="M56" s="11">
         <v>1</v>
       </c>
-      <c r="N56" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="O56" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P56" s="11" t="s">
-        <v>112</v>
+      <c r="N56" s="11">
+        <v>0</v>
+      </c>
+      <c r="O56" s="11">
+        <v>0</v>
+      </c>
+      <c r="P56" s="11">
+        <v>0</v>
       </c>
       <c r="Q56" s="11" t="s">
         <v>112</v>
@@ -11022,13 +11042,13 @@
         <v>112</v>
       </c>
       <c r="S56" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T56" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V56" s="11" t="s">
         <v>113</v>
@@ -11036,14 +11056,14 @@
       <c r="W56" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X56" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y56" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="11">
-        <v>0</v>
+      <c r="X56" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y56" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z56" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AA56" s="11">
         <v>0</v>
@@ -11117,14 +11137,14 @@
       <c r="M57" s="14">
         <v>1</v>
       </c>
-      <c r="N57" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O57" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P57" s="14" t="s">
-        <v>112</v>
+      <c r="N57" s="14">
+        <v>0</v>
+      </c>
+      <c r="O57" s="14">
+        <v>0</v>
+      </c>
+      <c r="P57" s="14">
+        <v>1</v>
       </c>
       <c r="Q57" s="14" t="s">
         <v>112</v>
@@ -11132,14 +11152,14 @@
       <c r="R57" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S57" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="T57" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="U57" s="14" t="s">
-        <v>113</v>
+      <c r="S57" t="s">
+        <v>112</v>
+      </c>
+      <c r="T57" t="s">
+        <v>112</v>
+      </c>
+      <c r="U57" t="s">
+        <v>112</v>
       </c>
       <c r="V57" s="14" t="s">
         <v>113</v>
@@ -11180,14 +11200,14 @@
       <c r="AH57" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AI57" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ57" s="14">
-        <v>0</v>
-      </c>
-      <c r="AK57" s="14">
-        <v>0</v>
+      <c r="AI57" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ57" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK57" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AL57" s="14">
         <v>0</v>
@@ -11464,14 +11484,14 @@
       <c r="M62" s="11">
         <v>0</v>
       </c>
-      <c r="N62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="O62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P62" s="11" t="s">
-        <v>112</v>
+      <c r="N62" s="11">
+        <v>0</v>
+      </c>
+      <c r="O62" s="11">
+        <v>0</v>
+      </c>
+      <c r="P62" s="11">
+        <v>0</v>
       </c>
       <c r="Q62" s="11" t="s">
         <v>112</v>
@@ -11480,13 +11500,13 @@
         <v>112</v>
       </c>
       <c r="S62" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T62" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V62" s="11" t="s">
         <v>113</v>
@@ -11494,14 +11514,14 @@
       <c r="W62" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X62" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="11">
-        <v>0</v>
+      <c r="X62" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y62" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z62" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AA62" s="11">
         <v>0</v>
@@ -11565,14 +11585,14 @@
       <c r="M63" s="14">
         <v>0</v>
       </c>
-      <c r="N63" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O63" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P63" s="14" t="s">
-        <v>112</v>
+      <c r="N63" s="14">
+        <v>0</v>
+      </c>
+      <c r="O63" s="14">
+        <v>0</v>
+      </c>
+      <c r="P63" s="14">
+        <v>1</v>
       </c>
       <c r="Q63" s="14" t="s">
         <v>112</v>
@@ -11580,14 +11600,14 @@
       <c r="R63" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S63" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="T63" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="U63" s="14" t="s">
-        <v>113</v>
+      <c r="S63" t="s">
+        <v>112</v>
+      </c>
+      <c r="T63" t="s">
+        <v>112</v>
+      </c>
+      <c r="U63" t="s">
+        <v>112</v>
       </c>
       <c r="V63" s="14" t="s">
         <v>113</v>
@@ -11628,14 +11648,14 @@
       <c r="AH63" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AI63" s="14">
-        <v>0</v>
-      </c>
-      <c r="AJ63" s="14">
-        <v>0</v>
-      </c>
-      <c r="AK63" s="14">
-        <v>0</v>
+      <c r="AI63" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ63" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK63" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AL63" s="14">
         <v>0</v>

</xml_diff>

<commit_message>
Updated values so that Destination Registers Line up
</commit_message>
<xml_diff>
--- a/Docs/MachineCode.xlsx
+++ b/Docs/MachineCode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="147">
   <si>
     <t>add</t>
   </si>
@@ -460,7 +460,7 @@
     <t>L = location</t>
   </si>
   <si>
-    <t>The grayed out ones are not yet implemented.</t>
+    <t>The grayed out ones are not yet determined.</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -748,8 +748,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -781,17 +801,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -840,6 +866,16 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -888,6 +924,16 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1217,28 +1263,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI78"/>
+  <dimension ref="A1:AI81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AG78"/>
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="33" width="2.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="8" width="2.83203125" style="14" customWidth="1"/>
+    <col min="9" max="33" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="10" t="s">
@@ -1254,10 +1301,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="11">
         <v>0</v>
@@ -1265,8 +1312,8 @@
       <c r="H2" s="11">
         <v>0</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>112</v>
+      <c r="I2" s="11">
+        <v>0</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>112</v>
@@ -1281,7 +1328,7 @@
         <v>112</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>113</v>
@@ -1295,8 +1342,8 @@
       <c r="R2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="S2" s="11">
-        <v>0</v>
+      <c r="S2" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="T2" s="11">
         <v>0</v>
@@ -1358,34 +1405,34 @@
         <v>0</v>
       </c>
       <c r="E3" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="14">
         <v>0</v>
       </c>
       <c r="H3" s="14">
-        <v>1</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="K3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>112</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>113</v>
@@ -1432,8 +1479,8 @@
       <c r="AC3" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AD3" s="14">
-        <v>0</v>
+      <c r="AD3" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AE3" s="14">
         <v>0</v>
@@ -1452,33 +1499,15 @@
       <c r="A4" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="17">
-        <v>0</v>
-      </c>
-      <c r="C4" s="17">
-        <v>0</v>
-      </c>
-      <c r="D4" s="17">
-        <v>0</v>
-      </c>
-      <c r="E4" s="17">
-        <v>1</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>112</v>
-      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
@@ -1510,18 +1539,10 @@
       <c r="A5" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="17">
-        <v>0</v>
-      </c>
-      <c r="C5" s="17">
-        <v>0</v>
-      </c>
-      <c r="D5" s="17">
-        <v>0</v>
-      </c>
-      <c r="E5" s="17">
-        <v>1</v>
-      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
@@ -1555,18 +1576,10 @@
       <c r="A6" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="17">
-        <v>0</v>
-      </c>
-      <c r="C6" s="17">
-        <v>0</v>
-      </c>
-      <c r="D6" s="17">
-        <v>0</v>
-      </c>
-      <c r="E6" s="17">
-        <v>1</v>
-      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -1603,18 +1616,10 @@
       <c r="A7" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="20">
-        <v>0</v>
-      </c>
-      <c r="C7" s="20">
-        <v>0</v>
-      </c>
-      <c r="D7" s="20">
-        <v>0</v>
-      </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -1655,10 +1660,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="11">
         <v>0</v>
@@ -1669,8 +1674,8 @@
       <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>112</v>
+      <c r="I8" s="11">
+        <v>0</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>112</v>
@@ -1685,7 +1690,7 @@
         <v>112</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O8" s="11" t="s">
         <v>113</v>
@@ -1699,8 +1704,8 @@
       <c r="R8" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="S8" s="11">
-        <v>0</v>
+      <c r="S8" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="T8" s="11">
         <v>0</v>
@@ -1756,10 +1761,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="14">
         <v>0</v>
@@ -1768,25 +1773,25 @@
         <v>0</v>
       </c>
       <c r="H9" s="14">
-        <v>1</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="K9" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>112</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O9" s="14" t="s">
         <v>113</v>
@@ -1833,8 +1838,8 @@
       <c r="AC9" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AD9" s="14">
-        <v>0</v>
+      <c r="AD9" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AE9" s="14">
         <v>0</v>
@@ -1850,33 +1855,15 @@
       <c r="A10" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="17">
-        <v>0</v>
-      </c>
-      <c r="C10" s="17">
-        <v>0</v>
-      </c>
-      <c r="D10" s="17">
-        <v>1</v>
-      </c>
-      <c r="E10" s="17">
-        <v>0</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>112</v>
-      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
@@ -1905,18 +1892,10 @@
       <c r="A11" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="17">
-        <v>0</v>
-      </c>
-      <c r="C11" s="17">
-        <v>0</v>
-      </c>
-      <c r="D11" s="17">
-        <v>1</v>
-      </c>
-      <c r="E11" s="17">
-        <v>0</v>
-      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -1950,18 +1929,10 @@
       <c r="A12" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="17">
-        <v>0</v>
-      </c>
-      <c r="C12" s="17">
-        <v>0</v>
-      </c>
-      <c r="D12" s="17">
-        <v>1</v>
-      </c>
-      <c r="E12" s="17">
-        <v>0</v>
-      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -1995,18 +1966,10 @@
       <c r="A13" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="20">
-        <v>0</v>
-      </c>
-      <c r="C13" s="20">
-        <v>0</v>
-      </c>
-      <c r="D13" s="20">
-        <v>1</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -2061,8 +2024,8 @@
       <c r="H14" s="11">
         <v>0</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>112</v>
+      <c r="I14" s="11">
+        <v>0</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>112</v>
@@ -2077,7 +2040,7 @@
         <v>112</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O14" s="11" t="s">
         <v>113</v>
@@ -2091,8 +2054,8 @@
       <c r="R14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="S14" s="11">
-        <v>0</v>
+      <c r="S14" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="T14" s="11">
         <v>0</v>
@@ -2160,25 +2123,25 @@
         <v>0</v>
       </c>
       <c r="H15" s="14">
-        <v>1</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1</v>
       </c>
       <c r="J15" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K15" t="s">
-        <v>112</v>
-      </c>
-      <c r="L15" t="s">
-        <v>112</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="K15" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="14" t="s">
         <v>112</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O15" s="14" t="s">
         <v>113</v>
@@ -2225,8 +2188,8 @@
       <c r="AC15" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AD15" s="14">
-        <v>0</v>
+      <c r="AD15" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AE15" s="14">
         <v>0</v>
@@ -2242,33 +2205,15 @@
       <c r="A16" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="17">
-        <v>0</v>
-      </c>
-      <c r="C16" s="17">
-        <v>0</v>
-      </c>
-      <c r="D16" s="17">
-        <v>0</v>
-      </c>
-      <c r="E16" s="17">
-        <v>0</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>112</v>
-      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
@@ -2297,18 +2242,10 @@
       <c r="A17" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="17">
-        <v>0</v>
-      </c>
-      <c r="D17" s="17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="17">
-        <v>0</v>
-      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -2342,18 +2279,10 @@
       <c r="A18" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="17">
-        <v>0</v>
-      </c>
-      <c r="C18" s="17">
-        <v>0</v>
-      </c>
-      <c r="D18" s="17">
-        <v>0</v>
-      </c>
-      <c r="E18" s="17">
-        <v>0</v>
-      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
@@ -2387,18 +2316,10 @@
       <c r="A19" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="20">
-        <v>0</v>
-      </c>
-      <c r="C19" s="20">
-        <v>0</v>
-      </c>
-      <c r="D19" s="20">
-        <v>0</v>
-      </c>
-      <c r="E19" s="20">
-        <v>0</v>
-      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -4561,42 +4482,42 @@
       <c r="E49" s="20">
         <v>1</v>
       </c>
-      <c r="F49" s="28">
-        <v>1</v>
-      </c>
-      <c r="G49" s="28">
-        <v>0</v>
-      </c>
-      <c r="H49" s="28">
-        <v>0</v>
-      </c>
-      <c r="I49" s="28">
-        <v>1</v>
-      </c>
-      <c r="J49" s="17"/>
-      <c r="K49" s="17"/>
-      <c r="L49" s="17"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-      <c r="P49" s="17"/>
-      <c r="Q49" s="17"/>
-      <c r="R49" s="17"/>
-      <c r="S49" s="17"/>
-      <c r="T49" s="17"/>
-      <c r="U49" s="17"/>
-      <c r="V49" s="17"/>
-      <c r="W49" s="17"/>
-      <c r="X49" s="17"/>
-      <c r="Y49" s="17"/>
-      <c r="Z49" s="17"/>
-      <c r="AA49" s="17"/>
-      <c r="AB49" s="17"/>
-      <c r="AC49" s="17"/>
-      <c r="AD49" s="17"/>
-      <c r="AE49" s="17"/>
-      <c r="AF49" s="17"/>
-      <c r="AG49" s="18"/>
+      <c r="F49" s="35">
+        <v>1</v>
+      </c>
+      <c r="G49" s="35">
+        <v>0</v>
+      </c>
+      <c r="H49" s="35">
+        <v>0</v>
+      </c>
+      <c r="I49" s="35">
+        <v>1</v>
+      </c>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="20"/>
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="20"/>
+      <c r="Z49" s="20"/>
+      <c r="AA49" s="20"/>
+      <c r="AB49" s="20"/>
+      <c r="AC49" s="20"/>
+      <c r="AD49" s="20"/>
+      <c r="AE49" s="20"/>
+      <c r="AF49" s="20"/>
+      <c r="AG49" s="21"/>
     </row>
     <row r="50" spans="1:33">
       <c r="A50" s="10" t="s">
@@ -4606,10 +4527,10 @@
         <v>0</v>
       </c>
       <c r="C50" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="11">
         <v>0</v>
@@ -4623,8 +4544,8 @@
       <c r="H50" s="11">
         <v>0</v>
       </c>
-      <c r="I50" s="11" t="s">
-        <v>112</v>
+      <c r="I50" s="11">
+        <v>0</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>112</v>
@@ -4639,7 +4560,7 @@
         <v>112</v>
       </c>
       <c r="N50" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O50" s="11" t="s">
         <v>113</v>
@@ -4653,8 +4574,8 @@
       <c r="R50" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="S50" s="11">
-        <v>0</v>
+      <c r="S50" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="T50" s="11">
         <v>0</v>
@@ -4707,10 +4628,10 @@
         <v>0</v>
       </c>
       <c r="C51" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" s="14">
         <v>0</v>
@@ -4722,25 +4643,25 @@
         <v>0</v>
       </c>
       <c r="H51" s="14">
-        <v>1</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="I51" s="14">
+        <v>1</v>
       </c>
       <c r="J51" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K51" t="s">
-        <v>112</v>
-      </c>
-      <c r="L51" t="s">
-        <v>112</v>
-      </c>
-      <c r="M51" t="s">
+      <c r="K51" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L51" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M51" s="14" t="s">
         <v>112</v>
       </c>
       <c r="N51" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O51" s="14" t="s">
         <v>113</v>
@@ -4787,8 +4708,8 @@
       <c r="AC51" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AD51" s="14">
-        <v>0</v>
+      <c r="AD51" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AE51" s="14">
         <v>0</v>
@@ -4804,33 +4725,15 @@
       <c r="A52" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="17">
-        <v>0</v>
-      </c>
-      <c r="C52" s="17">
-        <v>1</v>
-      </c>
-      <c r="D52" s="17">
-        <v>0</v>
-      </c>
-      <c r="E52" s="17">
-        <v>0</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I52" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>112</v>
-      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
@@ -4859,18 +4762,10 @@
       <c r="A53" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="17">
-        <v>0</v>
-      </c>
-      <c r="C53" s="17">
-        <v>1</v>
-      </c>
-      <c r="D53" s="17">
-        <v>0</v>
-      </c>
-      <c r="E53" s="17">
-        <v>0</v>
-      </c>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
@@ -4904,18 +4799,10 @@
       <c r="A54" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="17">
-        <v>0</v>
-      </c>
-      <c r="C54" s="17">
-        <v>1</v>
-      </c>
-      <c r="D54" s="17">
-        <v>0</v>
-      </c>
-      <c r="E54" s="17">
-        <v>0</v>
-      </c>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
@@ -4949,18 +4836,10 @@
       <c r="A55" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="20">
-        <v>0</v>
-      </c>
-      <c r="C55" s="20">
-        <v>1</v>
-      </c>
-      <c r="D55" s="20">
-        <v>0</v>
-      </c>
-      <c r="E55" s="20">
-        <v>0</v>
-      </c>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
@@ -4998,16 +4877,16 @@
         <v>0</v>
       </c>
       <c r="C56" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="11">
         <v>0</v>
@@ -5015,8 +4894,8 @@
       <c r="H56" s="11">
         <v>0</v>
       </c>
-      <c r="I56" s="11" t="s">
-        <v>112</v>
+      <c r="I56" s="11">
+        <v>0</v>
       </c>
       <c r="J56" s="11" t="s">
         <v>112</v>
@@ -5031,7 +4910,7 @@
         <v>112</v>
       </c>
       <c r="N56" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O56" s="11" t="s">
         <v>113</v>
@@ -5045,8 +4924,8 @@
       <c r="R56" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="S56" s="11">
-        <v>0</v>
+      <c r="S56" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="T56" s="11">
         <v>0</v>
@@ -5099,40 +4978,40 @@
         <v>0</v>
       </c>
       <c r="C57" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="14">
         <v>0</v>
       </c>
       <c r="H57" s="14">
-        <v>1</v>
-      </c>
-      <c r="I57" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="I57" s="14">
+        <v>1</v>
       </c>
       <c r="J57" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K57" t="s">
-        <v>112</v>
-      </c>
-      <c r="L57" t="s">
-        <v>112</v>
-      </c>
-      <c r="M57" t="s">
+      <c r="K57" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L57" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M57" s="14" t="s">
         <v>112</v>
       </c>
       <c r="N57" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O57" s="14" t="s">
         <v>113</v>
@@ -5179,8 +5058,8 @@
       <c r="AC57" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AD57" s="14">
-        <v>0</v>
+      <c r="AD57" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AE57" s="14">
         <v>0</v>
@@ -5196,33 +5075,15 @@
       <c r="A58" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B58" s="17">
-        <v>0</v>
-      </c>
-      <c r="C58" s="17">
-        <v>1</v>
-      </c>
-      <c r="D58" s="17">
-        <v>0</v>
-      </c>
-      <c r="E58" s="17">
-        <v>1</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H58" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I58" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J58" s="17" t="s">
-        <v>112</v>
-      </c>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
       <c r="K58" s="17"/>
       <c r="L58" s="17"/>
       <c r="M58" s="17"/>
@@ -5251,18 +5112,10 @@
       <c r="A59" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="17">
-        <v>0</v>
-      </c>
-      <c r="C59" s="17">
-        <v>1</v>
-      </c>
-      <c r="D59" s="17">
-        <v>0</v>
-      </c>
-      <c r="E59" s="17">
-        <v>1</v>
-      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
@@ -5296,18 +5149,10 @@
       <c r="A60" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B60" s="17">
-        <v>0</v>
-      </c>
-      <c r="C60" s="17">
-        <v>1</v>
-      </c>
-      <c r="D60" s="17">
-        <v>0</v>
-      </c>
-      <c r="E60" s="17">
-        <v>1</v>
-      </c>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -5341,18 +5186,10 @@
       <c r="A61" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B61" s="20">
-        <v>0</v>
-      </c>
-      <c r="C61" s="20">
-        <v>1</v>
-      </c>
-      <c r="D61" s="20">
-        <v>0</v>
-      </c>
-      <c r="E61" s="20">
-        <v>1</v>
-      </c>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
       <c r="F61" s="20"/>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
@@ -5383,103 +5220,103 @@
       <c r="AG61" s="21"/>
     </row>
     <row r="62" spans="1:33">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="11">
-        <v>0</v>
-      </c>
-      <c r="C62" s="11">
-        <v>1</v>
-      </c>
-      <c r="D62" s="11">
-        <v>1</v>
-      </c>
-      <c r="E62" s="11">
-        <v>0</v>
-      </c>
-      <c r="F62" s="11">
-        <v>0</v>
-      </c>
-      <c r="G62" s="11">
-        <v>0</v>
-      </c>
-      <c r="H62" s="11">
-        <v>0</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="J62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="K62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="L62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="M62" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="N62" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="O62" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="P62" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q62" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="R62" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="S62" s="11">
-        <v>0</v>
-      </c>
-      <c r="T62" s="11">
-        <v>0</v>
-      </c>
-      <c r="U62" s="11">
-        <v>0</v>
-      </c>
-      <c r="V62" s="11">
-        <v>0</v>
-      </c>
-      <c r="W62" s="11">
-        <v>0</v>
-      </c>
-      <c r="X62" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF62" s="11">
-        <v>0</v>
-      </c>
-      <c r="AG62" s="12">
+      <c r="B62" s="14">
+        <v>0</v>
+      </c>
+      <c r="C62" s="14">
+        <v>0</v>
+      </c>
+      <c r="D62" s="14">
+        <v>1</v>
+      </c>
+      <c r="E62" s="14">
+        <v>1</v>
+      </c>
+      <c r="F62" s="14">
+        <v>0</v>
+      </c>
+      <c r="G62" s="14">
+        <v>0</v>
+      </c>
+      <c r="H62" s="14">
+        <v>0</v>
+      </c>
+      <c r="I62" s="14">
+        <v>0</v>
+      </c>
+      <c r="J62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="N62" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="P62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="R62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="S62" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="T62" s="14">
+        <v>0</v>
+      </c>
+      <c r="U62" s="14">
+        <v>0</v>
+      </c>
+      <c r="V62" s="14">
+        <v>0</v>
+      </c>
+      <c r="W62" s="14">
+        <v>0</v>
+      </c>
+      <c r="X62" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF62" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="15">
         <v>0</v>
       </c>
     </row>
@@ -5491,13 +5328,13 @@
         <v>0</v>
       </c>
       <c r="C63" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="14">
         <v>1</v>
       </c>
       <c r="E63" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" s="14">
         <v>0</v>
@@ -5506,15 +5343,15 @@
         <v>0</v>
       </c>
       <c r="H63" s="14">
-        <v>1</v>
-      </c>
-      <c r="I63" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="I63" s="14">
+        <v>1</v>
       </c>
       <c r="J63" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K63" s="14" t="s">
         <v>112</v>
       </c>
       <c r="L63" t="s">
@@ -5523,8 +5360,8 @@
       <c r="M63" t="s">
         <v>112</v>
       </c>
-      <c r="N63" s="14" t="s">
-        <v>113</v>
+      <c r="N63" t="s">
+        <v>112</v>
       </c>
       <c r="O63" s="14" t="s">
         <v>113</v>
@@ -5571,8 +5408,8 @@
       <c r="AC63" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AD63" s="14">
-        <v>0</v>
+      <c r="AD63" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AE63" s="14">
         <v>0</v>
@@ -5588,33 +5425,15 @@
       <c r="A64" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="17">
-        <v>0</v>
-      </c>
-      <c r="C64" s="17">
-        <v>1</v>
-      </c>
-      <c r="D64" s="17">
-        <v>1</v>
-      </c>
-      <c r="E64" s="17">
-        <v>0</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G64" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I64" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J64" s="17" t="s">
-        <v>112</v>
-      </c>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
       <c r="K64" s="17"/>
       <c r="L64" s="17"/>
       <c r="M64" s="17"/>
@@ -5643,18 +5462,10 @@
       <c r="A65" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="17">
-        <v>0</v>
-      </c>
-      <c r="C65" s="17">
-        <v>1</v>
-      </c>
-      <c r="D65" s="17">
-        <v>1</v>
-      </c>
-      <c r="E65" s="17">
-        <v>0</v>
-      </c>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
@@ -5688,18 +5499,10 @@
       <c r="A66" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="17">
-        <v>0</v>
-      </c>
-      <c r="C66" s="17">
-        <v>1</v>
-      </c>
-      <c r="D66" s="17">
-        <v>1</v>
-      </c>
-      <c r="E66" s="17">
-        <v>0</v>
-      </c>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
       <c r="H66" s="17"/>
@@ -5730,49 +5533,41 @@
       <c r="AG66" s="18"/>
     </row>
     <row r="67" spans="1:33" ht="16" thickBot="1">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B67" s="20">
-        <v>0</v>
-      </c>
-      <c r="C67" s="20">
-        <v>1</v>
-      </c>
-      <c r="D67" s="20">
-        <v>1</v>
-      </c>
-      <c r="E67" s="20">
-        <v>0</v>
-      </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="20"/>
-      <c r="K67" s="20"/>
-      <c r="L67" s="20"/>
-      <c r="M67" s="20"/>
-      <c r="N67" s="20"/>
-      <c r="O67" s="20"/>
-      <c r="P67" s="20"/>
-      <c r="Q67" s="20"/>
-      <c r="R67" s="20"/>
-      <c r="S67" s="20"/>
-      <c r="T67" s="20"/>
-      <c r="U67" s="20"/>
-      <c r="V67" s="20"/>
-      <c r="W67" s="20"/>
-      <c r="X67" s="20"/>
-      <c r="Y67" s="20"/>
-      <c r="Z67" s="20"/>
-      <c r="AA67" s="20"/>
-      <c r="AB67" s="20"/>
-      <c r="AC67" s="20"/>
-      <c r="AD67" s="20"/>
-      <c r="AE67" s="20"/>
-      <c r="AF67" s="20"/>
-      <c r="AG67" s="21"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="17"/>
+      <c r="U67" s="17"/>
+      <c r="V67" s="17"/>
+      <c r="W67" s="17"/>
+      <c r="X67" s="17"/>
+      <c r="Y67" s="17"/>
+      <c r="Z67" s="17"/>
+      <c r="AA67" s="17"/>
+      <c r="AB67" s="17"/>
+      <c r="AC67" s="17"/>
+      <c r="AD67" s="17"/>
+      <c r="AE67" s="17"/>
+      <c r="AF67" s="17"/>
+      <c r="AG67" s="18"/>
     </row>
     <row r="68" spans="1:33">
       <c r="A68" s="22" t="s">
@@ -5782,25 +5577,25 @@
         <v>0</v>
       </c>
       <c r="C68" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="11">
         <v>1</v>
       </c>
       <c r="F68" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="11">
-        <v>0</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>112</v>
+        <v>1</v>
+      </c>
+      <c r="H68" s="11">
+        <v>0</v>
+      </c>
+      <c r="I68" s="11">
+        <v>0</v>
       </c>
       <c r="J68" s="11" t="s">
         <v>112</v>
@@ -5811,8 +5606,12 @@
       <c r="L68" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M68" s="11"/>
-      <c r="N68" s="11"/>
+      <c r="M68" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N68" s="11" t="s">
+        <v>112</v>
+      </c>
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
       <c r="Q68" s="11"/>
@@ -5837,41 +5636,19 @@
       <c r="A69" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B69" s="17">
-        <v>0</v>
-      </c>
-      <c r="C69" s="17">
-        <v>1</v>
-      </c>
-      <c r="D69" s="17">
-        <v>1</v>
-      </c>
-      <c r="E69" s="17">
-        <v>1</v>
-      </c>
-      <c r="F69" s="28">
-        <v>0</v>
-      </c>
-      <c r="G69" s="28">
-        <v>0</v>
-      </c>
-      <c r="H69" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I69" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J69" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K69" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="L69" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
       <c r="O69" s="17"/>
       <c r="P69" s="17"/>
       <c r="Q69" s="17"/>
@@ -5900,37 +5677,41 @@
         <v>0</v>
       </c>
       <c r="C70" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" s="14">
         <v>1</v>
       </c>
-      <c r="F70" s="27">
-        <v>0</v>
-      </c>
-      <c r="G70" s="27">
-        <v>1</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="I70" s="14" t="s">
-        <v>112</v>
+      <c r="F70" s="14">
+        <v>1</v>
+      </c>
+      <c r="G70" s="14">
+        <v>1</v>
+      </c>
+      <c r="H70" s="27">
+        <v>0</v>
+      </c>
+      <c r="I70" s="27">
+        <v>1</v>
       </c>
       <c r="J70" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K70" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="L70" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="M70" s="14"/>
-      <c r="N70" s="14"/>
+      <c r="K70" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L70" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M70" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="N70" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="O70" s="14"/>
       <c r="P70" s="14"/>
       <c r="Q70" s="14"/>
@@ -5955,41 +5736,19 @@
       <c r="A71" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B71" s="17">
-        <v>0</v>
-      </c>
-      <c r="C71" s="17">
-        <v>1</v>
-      </c>
-      <c r="D71" s="17">
-        <v>1</v>
-      </c>
-      <c r="E71" s="17">
-        <v>1</v>
-      </c>
-      <c r="F71" s="28">
-        <v>0</v>
-      </c>
-      <c r="G71" s="28">
-        <v>1</v>
-      </c>
-      <c r="H71" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I71" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J71" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K71" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="L71" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="17"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="28"/>
       <c r="O71" s="17"/>
       <c r="P71" s="17"/>
       <c r="Q71" s="17"/>
@@ -6018,37 +5777,41 @@
         <v>0</v>
       </c>
       <c r="C72" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" s="14">
         <v>1</v>
       </c>
-      <c r="F72" s="27">
-        <v>1</v>
-      </c>
-      <c r="G72" s="27">
-        <v>0</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="I72" s="14" t="s">
-        <v>112</v>
+      <c r="F72" s="14">
+        <v>1</v>
+      </c>
+      <c r="G72" s="14">
+        <v>1</v>
+      </c>
+      <c r="H72" s="27">
+        <v>1</v>
+      </c>
+      <c r="I72" s="27">
+        <v>0</v>
       </c>
       <c r="J72" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K72" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="L72" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
+      <c r="K72" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L72" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M72" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="N72" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="O72" s="14"/>
       <c r="P72" s="14"/>
       <c r="Q72" s="14"/>
@@ -6073,41 +5836,19 @@
       <c r="A73" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="17">
-        <v>0</v>
-      </c>
-      <c r="C73" s="17">
-        <v>1</v>
-      </c>
-      <c r="D73" s="17">
-        <v>1</v>
-      </c>
-      <c r="E73" s="17">
-        <v>1</v>
-      </c>
-      <c r="F73" s="28">
-        <v>1</v>
-      </c>
-      <c r="G73" s="28">
-        <v>0</v>
-      </c>
-      <c r="H73" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I73" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J73" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K73" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="L73" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="28"/>
       <c r="O73" s="17"/>
       <c r="P73" s="17"/>
       <c r="Q73" s="17"/>
@@ -6136,37 +5877,41 @@
         <v>0</v>
       </c>
       <c r="C74" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="14">
         <v>1</v>
       </c>
-      <c r="F74" s="27">
-        <v>1</v>
-      </c>
-      <c r="G74" s="27">
-        <v>1</v>
-      </c>
-      <c r="H74" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="I74" s="14" t="s">
-        <v>112</v>
+      <c r="F74" s="14">
+        <v>1</v>
+      </c>
+      <c r="G74" s="14">
+        <v>1</v>
+      </c>
+      <c r="H74" s="27">
+        <v>1</v>
+      </c>
+      <c r="I74" s="27">
+        <v>1</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K74" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="L74" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="M74" s="14"/>
-      <c r="N74" s="14"/>
+      <c r="K74" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L74" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M74" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="N74" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="O74" s="14"/>
       <c r="P74" s="14"/>
       <c r="Q74" s="14"/>
@@ -6191,41 +5936,19 @@
       <c r="A75" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B75" s="20">
-        <v>0</v>
-      </c>
-      <c r="C75" s="20">
-        <v>1</v>
-      </c>
-      <c r="D75" s="20">
-        <v>1</v>
-      </c>
-      <c r="E75" s="20">
-        <v>1</v>
-      </c>
-      <c r="F75" s="20">
-        <v>1</v>
-      </c>
-      <c r="G75" s="20">
-        <v>1</v>
-      </c>
-      <c r="H75" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I75" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J75" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K75" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="L75" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="M75" s="20"/>
-      <c r="N75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="35"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="20"/>
+      <c r="M75" s="35"/>
+      <c r="N75" s="35"/>
       <c r="O75" s="20"/>
       <c r="P75" s="20"/>
       <c r="Q75" s="20"/>
@@ -6247,103 +5970,103 @@
       <c r="AG75" s="21"/>
     </row>
     <row r="76" spans="1:33" ht="16" thickBot="1">
-      <c r="A76" s="24" t="s">
+      <c r="A76" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B76" s="25">
-        <v>1</v>
-      </c>
-      <c r="C76" s="25">
-        <v>0</v>
-      </c>
-      <c r="D76" s="25">
-        <v>0</v>
-      </c>
-      <c r="E76" s="25">
-        <v>0</v>
-      </c>
-      <c r="F76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="H76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="I76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="J76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="K76" s="11">
-        <v>0</v>
-      </c>
-      <c r="L76" s="11">
-        <v>0</v>
-      </c>
-      <c r="M76" s="11">
-        <v>0</v>
-      </c>
-      <c r="N76" s="11">
-        <v>0</v>
-      </c>
-      <c r="O76" s="11">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q76" s="11">
-        <v>0</v>
-      </c>
-      <c r="R76" s="11">
-        <v>0</v>
-      </c>
-      <c r="S76" s="11">
-        <v>0</v>
-      </c>
-      <c r="T76" s="11">
-        <v>0</v>
-      </c>
-      <c r="U76" s="11">
-        <v>0</v>
-      </c>
-      <c r="V76" s="11">
-        <v>0</v>
-      </c>
-      <c r="W76" s="11">
-        <v>0</v>
-      </c>
-      <c r="X76" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y76" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF76" s="11">
-        <v>0</v>
-      </c>
-      <c r="AG76" s="12">
+      <c r="B76" s="29">
+        <v>0</v>
+      </c>
+      <c r="C76" s="29">
+        <v>0</v>
+      </c>
+      <c r="D76" s="29">
+        <v>0</v>
+      </c>
+      <c r="E76" s="29">
+        <v>0</v>
+      </c>
+      <c r="F76" s="14">
+        <v>1</v>
+      </c>
+      <c r="G76" s="14">
+        <v>0</v>
+      </c>
+      <c r="H76" s="14">
+        <v>0</v>
+      </c>
+      <c r="I76" s="14">
+        <v>0</v>
+      </c>
+      <c r="J76" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="L76" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="M76" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="N76" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="O76" s="14">
+        <v>0</v>
+      </c>
+      <c r="P76" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="14">
+        <v>0</v>
+      </c>
+      <c r="R76" s="14">
+        <v>0</v>
+      </c>
+      <c r="S76" s="14">
+        <v>0</v>
+      </c>
+      <c r="T76" s="14">
+        <v>0</v>
+      </c>
+      <c r="U76" s="14">
+        <v>0</v>
+      </c>
+      <c r="V76" s="14">
+        <v>0</v>
+      </c>
+      <c r="W76" s="14">
+        <v>0</v>
+      </c>
+      <c r="X76" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y76" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF76" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG76" s="15">
         <v>0</v>
       </c>
     </row>
@@ -6351,201 +6074,504 @@
       <c r="A77" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="25">
-        <v>1</v>
-      </c>
-      <c r="C77" s="25">
-        <v>0</v>
-      </c>
-      <c r="D77" s="25">
-        <v>0</v>
-      </c>
-      <c r="E77" s="25">
-        <v>1</v>
-      </c>
-      <c r="F77" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G77" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="H77" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="I77" s="25" t="s">
-        <v>113</v>
+      <c r="B77" s="33">
+        <v>0</v>
+      </c>
+      <c r="C77" s="33">
+        <v>0</v>
+      </c>
+      <c r="D77" s="33">
+        <v>0</v>
+      </c>
+      <c r="E77" s="33">
+        <v>0</v>
+      </c>
+      <c r="F77" s="25">
+        <v>1</v>
+      </c>
+      <c r="G77" s="25">
+        <v>0</v>
+      </c>
+      <c r="H77" s="25">
+        <v>0</v>
+      </c>
+      <c r="I77" s="25">
+        <v>1</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K77" s="11">
-        <v>0</v>
-      </c>
-      <c r="L77" s="11">
-        <v>0</v>
-      </c>
-      <c r="M77" s="11">
-        <v>0</v>
-      </c>
-      <c r="N77" s="11">
-        <v>0</v>
-      </c>
-      <c r="O77" s="11">
-        <v>0</v>
-      </c>
-      <c r="P77" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q77" s="11">
-        <v>0</v>
-      </c>
-      <c r="R77" s="11">
-        <v>0</v>
-      </c>
-      <c r="S77" s="11">
-        <v>0</v>
-      </c>
-      <c r="T77" s="11">
-        <v>0</v>
-      </c>
-      <c r="U77" s="11">
-        <v>0</v>
-      </c>
-      <c r="V77" s="11">
-        <v>0</v>
-      </c>
-      <c r="W77" s="11">
-        <v>0</v>
-      </c>
-      <c r="X77" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y77" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AF77" s="11">
-        <v>0</v>
-      </c>
-      <c r="AG77" s="12">
+      <c r="K77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="L77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="M77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="N77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="O77" s="25">
+        <v>0</v>
+      </c>
+      <c r="P77" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="25">
+        <v>0</v>
+      </c>
+      <c r="R77" s="25">
+        <v>0</v>
+      </c>
+      <c r="S77" s="25">
+        <v>0</v>
+      </c>
+      <c r="T77" s="25">
+        <v>0</v>
+      </c>
+      <c r="U77" s="25">
+        <v>0</v>
+      </c>
+      <c r="V77" s="25">
+        <v>0</v>
+      </c>
+      <c r="W77" s="25">
+        <v>0</v>
+      </c>
+      <c r="X77" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y77" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AC77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AF77" s="25">
+        <v>0</v>
+      </c>
+      <c r="AG77" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:33" ht="16" thickBot="1">
-      <c r="A78" s="24" t="s">
+      <c r="A78" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B78" s="25">
-        <v>1</v>
-      </c>
-      <c r="C78" s="25">
-        <v>0</v>
-      </c>
-      <c r="D78" s="25">
-        <v>1</v>
-      </c>
-      <c r="E78" s="25">
-        <v>0</v>
-      </c>
-      <c r="F78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="H78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="I78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="J78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="K78" s="25">
-        <v>0</v>
-      </c>
-      <c r="L78" s="25">
-        <v>0</v>
-      </c>
-      <c r="M78" s="25">
-        <v>0</v>
-      </c>
-      <c r="N78" s="25">
-        <v>0</v>
-      </c>
-      <c r="O78" s="25">
-        <v>0</v>
-      </c>
-      <c r="P78" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q78" s="25">
-        <v>0</v>
-      </c>
-      <c r="R78" s="25">
-        <v>0</v>
-      </c>
-      <c r="S78" s="25">
-        <v>0</v>
-      </c>
-      <c r="T78" s="25">
-        <v>0</v>
-      </c>
-      <c r="U78" s="25">
-        <v>0</v>
-      </c>
-      <c r="V78" s="25">
-        <v>0</v>
-      </c>
-      <c r="W78" s="25">
-        <v>0</v>
-      </c>
-      <c r="X78" s="25">
-        <v>0</v>
-      </c>
-      <c r="Y78" s="25">
-        <v>0</v>
-      </c>
-      <c r="Z78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AA78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AB78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AC78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AD78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AE78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AF78" s="25">
-        <v>0</v>
-      </c>
-      <c r="AG78" s="26">
+      <c r="B78" s="29">
+        <v>0</v>
+      </c>
+      <c r="C78" s="29">
+        <v>0</v>
+      </c>
+      <c r="D78" s="29">
+        <v>0</v>
+      </c>
+      <c r="E78" s="29">
+        <v>0</v>
+      </c>
+      <c r="F78" s="14">
+        <v>1</v>
+      </c>
+      <c r="G78" s="14">
+        <v>0</v>
+      </c>
+      <c r="H78" s="14">
+        <v>1</v>
+      </c>
+      <c r="I78" s="14">
+        <v>0</v>
+      </c>
+      <c r="J78" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K78" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L78" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M78" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="N78" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O78" s="14">
+        <v>0</v>
+      </c>
+      <c r="P78" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="14">
+        <v>0</v>
+      </c>
+      <c r="R78" s="14">
+        <v>0</v>
+      </c>
+      <c r="S78" s="14">
+        <v>0</v>
+      </c>
+      <c r="T78" s="14">
+        <v>0</v>
+      </c>
+      <c r="U78" s="14">
+        <v>0</v>
+      </c>
+      <c r="V78" s="14">
+        <v>0</v>
+      </c>
+      <c r="W78" s="14">
+        <v>0</v>
+      </c>
+      <c r="X78" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG78" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:33" ht="16" thickBot="1">
+      <c r="A79" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B79" s="25">
+        <v>1</v>
+      </c>
+      <c r="C79" s="25">
+        <v>0</v>
+      </c>
+      <c r="D79" s="25">
+        <v>0</v>
+      </c>
+      <c r="E79" s="25">
+        <v>0</v>
+      </c>
+      <c r="F79" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G79" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="H79" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="I79" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J79" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K79" s="25">
+        <v>0</v>
+      </c>
+      <c r="L79" s="25">
+        <v>0</v>
+      </c>
+      <c r="M79" s="25">
+        <v>0</v>
+      </c>
+      <c r="N79" s="25">
+        <v>0</v>
+      </c>
+      <c r="O79" s="25">
+        <v>0</v>
+      </c>
+      <c r="P79" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="25">
+        <v>0</v>
+      </c>
+      <c r="R79" s="25">
+        <v>0</v>
+      </c>
+      <c r="S79" s="25">
+        <v>0</v>
+      </c>
+      <c r="T79" s="25">
+        <v>0</v>
+      </c>
+      <c r="U79" s="25">
+        <v>0</v>
+      </c>
+      <c r="V79" s="25">
+        <v>0</v>
+      </c>
+      <c r="W79" s="25">
+        <v>0</v>
+      </c>
+      <c r="X79" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y79" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AC79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AF79" s="25">
+        <v>0</v>
+      </c>
+      <c r="AG79" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:33" ht="16" thickBot="1">
+      <c r="A80" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80" s="14">
+        <v>1</v>
+      </c>
+      <c r="C80" s="14">
+        <v>0</v>
+      </c>
+      <c r="D80" s="14">
+        <v>0</v>
+      </c>
+      <c r="E80" s="14">
+        <v>1</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="J80" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K80" s="14">
+        <v>0</v>
+      </c>
+      <c r="L80" s="14">
+        <v>0</v>
+      </c>
+      <c r="M80" s="14">
+        <v>0</v>
+      </c>
+      <c r="N80" s="14">
+        <v>0</v>
+      </c>
+      <c r="O80" s="14">
+        <v>0</v>
+      </c>
+      <c r="P80" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="14">
+        <v>0</v>
+      </c>
+      <c r="R80" s="14">
+        <v>0</v>
+      </c>
+      <c r="S80" s="14">
+        <v>0</v>
+      </c>
+      <c r="T80" s="14">
+        <v>0</v>
+      </c>
+      <c r="U80" s="14">
+        <v>0</v>
+      </c>
+      <c r="V80" s="14">
+        <v>0</v>
+      </c>
+      <c r="W80" s="14">
+        <v>0</v>
+      </c>
+      <c r="X80" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y80" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF80" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG80" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:33" ht="16" thickBot="1">
+      <c r="A81" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" s="25">
+        <v>1</v>
+      </c>
+      <c r="C81" s="25">
+        <v>0</v>
+      </c>
+      <c r="D81" s="25">
+        <v>1</v>
+      </c>
+      <c r="E81" s="25">
+        <v>0</v>
+      </c>
+      <c r="F81" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G81" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H81" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I81" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="J81" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="K81" s="25">
+        <v>0</v>
+      </c>
+      <c r="L81" s="25">
+        <v>0</v>
+      </c>
+      <c r="M81" s="25">
+        <v>0</v>
+      </c>
+      <c r="N81" s="25">
+        <v>0</v>
+      </c>
+      <c r="O81" s="25">
+        <v>0</v>
+      </c>
+      <c r="P81" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="25">
+        <v>0</v>
+      </c>
+      <c r="R81" s="25">
+        <v>0</v>
+      </c>
+      <c r="S81" s="25">
+        <v>0</v>
+      </c>
+      <c r="T81" s="25">
+        <v>0</v>
+      </c>
+      <c r="U81" s="25">
+        <v>0</v>
+      </c>
+      <c r="V81" s="25">
+        <v>0</v>
+      </c>
+      <c r="W81" s="25">
+        <v>0</v>
+      </c>
+      <c r="X81" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y81" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AC81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AF81" s="25">
+        <v>0</v>
+      </c>
+      <c r="AG81" s="26">
         <v>0</v>
       </c>
     </row>
@@ -6567,7 +6593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:AO78"/>
     </sheetView>
   </sheetViews>
@@ -6585,12 +6611,16 @@
       <c r="I1" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:41">
       <c r="A2" t="s">
@@ -6615,10 +6645,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="11">
         <v>0</v>
@@ -6626,8 +6656,8 @@
       <c r="P2" s="11">
         <v>0</v>
       </c>
-      <c r="Q2" s="11" t="s">
-        <v>112</v>
+      <c r="Q2" s="11">
+        <v>0</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>112</v>
@@ -6642,7 +6672,7 @@
         <v>112</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W2" s="11" t="s">
         <v>113</v>
@@ -6656,8 +6686,8 @@
       <c r="Z2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AA2" s="11">
-        <v>0</v>
+      <c r="AA2" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AB2" s="11">
         <v>0</v>
@@ -6734,24 +6764,24 @@
         <v>0</v>
       </c>
       <c r="M3" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="14">
         <v>0</v>
       </c>
       <c r="P3" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>1</v>
       </c>
       <c r="R3" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="14" t="s">
         <v>112</v>
       </c>
       <c r="T3" t="s">
@@ -6760,8 +6790,8 @@
       <c r="U3" t="s">
         <v>112</v>
       </c>
-      <c r="V3" s="14" t="s">
-        <v>113</v>
+      <c r="V3" t="s">
+        <v>112</v>
       </c>
       <c r="W3" s="14" t="s">
         <v>113</v>
@@ -6808,8 +6838,8 @@
       <c r="AK3" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AL3" s="14">
-        <v>0</v>
+      <c r="AL3" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AM3" s="14">
         <v>0</v>
@@ -6853,10 +6883,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="17">
-        <v>1</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="N4" s="17">
+        <v>1</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>112</v>
@@ -6870,7 +6900,9 @@
       <c r="R4" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S4" s="17"/>
+      <c r="S4" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="T4" s="17"/>
       <c r="U4" s="17"/>
       <c r="V4" s="17"/>
@@ -6917,9 +6949,11 @@
         <v>0</v>
       </c>
       <c r="M5" s="17">
-        <v>1</v>
-      </c>
-      <c r="N5" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="17">
+        <v>1</v>
+      </c>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
@@ -6971,9 +7005,11 @@
         <v>0</v>
       </c>
       <c r="M6" s="17">
-        <v>1</v>
-      </c>
-      <c r="N6" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="17">
+        <v>1</v>
+      </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
@@ -7025,9 +7061,11 @@
         <v>0</v>
       </c>
       <c r="M7" s="20">
-        <v>1</v>
-      </c>
-      <c r="N7" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
+        <v>1</v>
+      </c>
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
@@ -7076,10 +7114,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="11">
         <v>0</v>
@@ -7090,8 +7128,8 @@
       <c r="P8" s="11">
         <v>0</v>
       </c>
-      <c r="Q8" s="11" t="s">
-        <v>112</v>
+      <c r="Q8" s="11">
+        <v>0</v>
       </c>
       <c r="R8" s="11" t="s">
         <v>112</v>
@@ -7106,7 +7144,7 @@
         <v>112</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W8" s="11" t="s">
         <v>113</v>
@@ -7120,8 +7158,8 @@
       <c r="Z8" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AA8" s="11">
-        <v>0</v>
+      <c r="AA8" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AB8" s="11">
         <v>0</v>
@@ -7186,10 +7224,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="14">
         <v>0</v>
@@ -7198,15 +7236,15 @@
         <v>0</v>
       </c>
       <c r="P9" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>1</v>
       </c>
       <c r="R9" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="14" t="s">
         <v>112</v>
       </c>
       <c r="T9" t="s">
@@ -7215,8 +7253,8 @@
       <c r="U9" t="s">
         <v>112</v>
       </c>
-      <c r="V9" s="14" t="s">
-        <v>113</v>
+      <c r="V9" t="s">
+        <v>112</v>
       </c>
       <c r="W9" s="14" t="s">
         <v>113</v>
@@ -7263,8 +7301,8 @@
       <c r="AK9" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AL9" s="14">
-        <v>0</v>
+      <c r="AL9" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AM9" s="14">
         <v>0</v>
@@ -7305,13 +7343,13 @@
         <v>0</v>
       </c>
       <c r="L10" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="17">
-        <v>0</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>112</v>
+        <v>1</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0</v>
       </c>
       <c r="O10" s="17" t="s">
         <v>112</v>
@@ -7325,7 +7363,9 @@
       <c r="R10" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S10" s="17"/>
+      <c r="S10" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
@@ -7378,12 +7418,14 @@
         <v>0</v>
       </c>
       <c r="L11" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="17">
-        <v>0</v>
-      </c>
-      <c r="N11" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
@@ -7432,12 +7474,14 @@
         <v>0</v>
       </c>
       <c r="L12" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="17">
-        <v>0</v>
-      </c>
-      <c r="N12" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="17">
+        <v>0</v>
+      </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
@@ -7486,12 +7530,14 @@
         <v>0</v>
       </c>
       <c r="L13" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="20">
-        <v>0</v>
-      </c>
-      <c r="N13" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="N13" s="20">
+        <v>0</v>
+      </c>
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
@@ -7554,8 +7600,8 @@
       <c r="P14" s="11">
         <v>0</v>
       </c>
-      <c r="Q14" s="11" t="s">
-        <v>112</v>
+      <c r="Q14" s="11">
+        <v>0</v>
       </c>
       <c r="R14" s="11" t="s">
         <v>112</v>
@@ -7570,7 +7616,7 @@
         <v>112</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W14" s="11" t="s">
         <v>113</v>
@@ -7584,8 +7630,8 @@
       <c r="Z14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AA14" s="11">
-        <v>0</v>
+      <c r="AA14" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AB14" s="11">
         <v>0</v>
@@ -7662,15 +7708,15 @@
         <v>0</v>
       </c>
       <c r="P15" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>1</v>
       </c>
       <c r="R15" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S15" s="14" t="s">
         <v>112</v>
       </c>
       <c r="T15" t="s">
@@ -7679,8 +7725,8 @@
       <c r="U15" t="s">
         <v>112</v>
       </c>
-      <c r="V15" s="14" t="s">
-        <v>113</v>
+      <c r="V15" t="s">
+        <v>112</v>
       </c>
       <c r="W15" s="14" t="s">
         <v>113</v>
@@ -7727,8 +7773,8 @@
       <c r="AK15" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AL15" s="14">
-        <v>0</v>
+      <c r="AL15" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AM15" s="14">
         <v>0</v>
@@ -7775,8 +7821,8 @@
       <c r="M16" s="17">
         <v>0</v>
       </c>
-      <c r="N16" s="17" t="s">
-        <v>112</v>
+      <c r="N16" s="17">
+        <v>0</v>
       </c>
       <c r="O16" s="17" t="s">
         <v>112</v>
@@ -7790,7 +7836,9 @@
       <c r="R16" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S16" s="17"/>
+      <c r="S16" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="T16" s="17"/>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
@@ -7849,7 +7897,9 @@
       <c r="M17" s="17">
         <v>0</v>
       </c>
-      <c r="N17" s="17"/>
+      <c r="N17" s="17">
+        <v>0</v>
+      </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
@@ -7904,7 +7954,9 @@
       <c r="M18" s="17">
         <v>0</v>
       </c>
-      <c r="N18" s="17"/>
+      <c r="N18" s="17">
+        <v>0</v>
+      </c>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="17"/>
@@ -7959,7 +8011,9 @@
       <c r="M19" s="20">
         <v>0</v>
       </c>
-      <c r="N19" s="20"/>
+      <c r="N19" s="20">
+        <v>0</v>
+      </c>
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
@@ -10563,10 +10617,10 @@
         <v>0</v>
       </c>
       <c r="K50" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="11">
         <v>0</v>
@@ -10580,8 +10634,8 @@
       <c r="P50" s="11">
         <v>0</v>
       </c>
-      <c r="Q50" s="11" t="s">
-        <v>112</v>
+      <c r="Q50" s="11">
+        <v>0</v>
       </c>
       <c r="R50" s="11" t="s">
         <v>112</v>
@@ -10596,7 +10650,7 @@
         <v>112</v>
       </c>
       <c r="V50" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W50" s="11" t="s">
         <v>113</v>
@@ -10610,8 +10664,8 @@
       <c r="Z50" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AA50" s="11">
-        <v>0</v>
+      <c r="AA50" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AB50" s="11">
         <v>0</v>
@@ -10676,10 +10730,10 @@
         <v>0</v>
       </c>
       <c r="K51" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="14">
         <v>0</v>
@@ -10691,15 +10745,15 @@
         <v>0</v>
       </c>
       <c r="P51" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="Q51" s="14">
+        <v>1</v>
       </c>
       <c r="R51" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S51" t="s">
+      <c r="S51" s="14" t="s">
         <v>112</v>
       </c>
       <c r="T51" t="s">
@@ -10708,8 +10762,8 @@
       <c r="U51" t="s">
         <v>112</v>
       </c>
-      <c r="V51" s="14" t="s">
-        <v>113</v>
+      <c r="V51" t="s">
+        <v>112</v>
       </c>
       <c r="W51" s="14" t="s">
         <v>113</v>
@@ -10756,8 +10810,8 @@
       <c r="AK51" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AL51" s="14">
-        <v>0</v>
+      <c r="AL51" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AM51" s="14">
         <v>0</v>
@@ -10789,16 +10843,16 @@
         <v>0</v>
       </c>
       <c r="K52" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" s="17">
         <v>0</v>
       </c>
-      <c r="N52" s="17" t="s">
-        <v>112</v>
+      <c r="N52" s="17">
+        <v>0</v>
       </c>
       <c r="O52" s="17" t="s">
         <v>112</v>
@@ -10812,7 +10866,9 @@
       <c r="R52" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S52" s="17"/>
+      <c r="S52" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="T52" s="17"/>
       <c r="U52" s="17"/>
       <c r="V52" s="17"/>
@@ -10856,15 +10912,17 @@
         <v>0</v>
       </c>
       <c r="K53" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" s="17">
         <v>0</v>
       </c>
-      <c r="N53" s="17"/>
+      <c r="N53" s="17">
+        <v>0</v>
+      </c>
       <c r="O53" s="17"/>
       <c r="P53" s="17"/>
       <c r="Q53" s="17"/>
@@ -10913,15 +10971,17 @@
         <v>0</v>
       </c>
       <c r="K54" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" s="17">
         <v>0</v>
       </c>
-      <c r="N54" s="17"/>
+      <c r="N54" s="17">
+        <v>0</v>
+      </c>
       <c r="O54" s="17"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="17"/>
@@ -10967,15 +11027,17 @@
         <v>0</v>
       </c>
       <c r="K55" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M55" s="20">
         <v>0</v>
       </c>
-      <c r="N55" s="20"/>
+      <c r="N55" s="20">
+        <v>0</v>
+      </c>
       <c r="O55" s="20"/>
       <c r="P55" s="20"/>
       <c r="Q55" s="20"/>
@@ -11022,16 +11084,16 @@
         <v>0</v>
       </c>
       <c r="K56" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" s="11">
         <v>0</v>
@@ -11039,8 +11101,8 @@
       <c r="P56" s="11">
         <v>0</v>
       </c>
-      <c r="Q56" s="11" t="s">
-        <v>112</v>
+      <c r="Q56" s="11">
+        <v>0</v>
       </c>
       <c r="R56" s="11" t="s">
         <v>112</v>
@@ -11055,7 +11117,7 @@
         <v>112</v>
       </c>
       <c r="V56" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W56" s="11" t="s">
         <v>113</v>
@@ -11069,8 +11131,8 @@
       <c r="Z56" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AA56" s="11">
-        <v>0</v>
+      <c r="AA56" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AB56" s="11">
         <v>0</v>
@@ -11133,30 +11195,30 @@
         <v>0</v>
       </c>
       <c r="K57" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M57" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N57" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57" s="14">
         <v>0</v>
       </c>
       <c r="P57" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q57" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="Q57" s="14">
+        <v>1</v>
       </c>
       <c r="R57" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S57" t="s">
+      <c r="S57" s="14" t="s">
         <v>112</v>
       </c>
       <c r="T57" t="s">
@@ -11165,8 +11227,8 @@
       <c r="U57" t="s">
         <v>112</v>
       </c>
-      <c r="V57" s="14" t="s">
-        <v>113</v>
+      <c r="V57" t="s">
+        <v>112</v>
       </c>
       <c r="W57" s="14" t="s">
         <v>113</v>
@@ -11213,8 +11275,8 @@
       <c r="AK57" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AL57" s="14">
-        <v>0</v>
+      <c r="AL57" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AM57" s="14">
         <v>0</v>
@@ -11244,16 +11306,16 @@
         <v>0</v>
       </c>
       <c r="K58" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L58" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M58" s="17">
-        <v>1</v>
-      </c>
-      <c r="N58" s="17" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="N58" s="17">
+        <v>1</v>
       </c>
       <c r="O58" s="17" t="s">
         <v>112</v>
@@ -11267,7 +11329,9 @@
       <c r="R58" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S58" s="17"/>
+      <c r="S58" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="T58" s="17"/>
       <c r="U58" s="17"/>
       <c r="V58" s="17"/>
@@ -11309,15 +11373,17 @@
         <v>0</v>
       </c>
       <c r="K59" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="17">
-        <v>1</v>
-      </c>
-      <c r="N59" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="N59" s="17">
+        <v>1</v>
+      </c>
       <c r="O59" s="17"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="17"/>
@@ -11366,15 +11432,17 @@
         <v>0</v>
       </c>
       <c r="K60" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" s="17">
-        <v>1</v>
-      </c>
-      <c r="N60" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="N60" s="17">
+        <v>1</v>
+      </c>
       <c r="O60" s="17"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="17"/>
@@ -11423,15 +11491,17 @@
         <v>0</v>
       </c>
       <c r="K61" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" s="20">
-        <v>1</v>
-      </c>
-      <c r="N61" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="N61" s="20">
+        <v>1</v>
+      </c>
       <c r="O61" s="20"/>
       <c r="P61" s="20"/>
       <c r="Q61" s="20"/>
@@ -11480,13 +11550,13 @@
         <v>0</v>
       </c>
       <c r="K62" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L62" s="11">
         <v>1</v>
       </c>
       <c r="M62" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N62" s="11">
         <v>0</v>
@@ -11497,8 +11567,8 @@
       <c r="P62" s="11">
         <v>0</v>
       </c>
-      <c r="Q62" s="11" t="s">
-        <v>112</v>
+      <c r="Q62" s="11">
+        <v>0</v>
       </c>
       <c r="R62" s="11" t="s">
         <v>112</v>
@@ -11513,7 +11583,7 @@
         <v>112</v>
       </c>
       <c r="V62" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W62" s="11" t="s">
         <v>113</v>
@@ -11527,8 +11597,8 @@
       <c r="Z62" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AA62" s="11">
-        <v>0</v>
+      <c r="AA62" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="AB62" s="11">
         <v>0</v>
@@ -11581,13 +11651,13 @@
         <v>0</v>
       </c>
       <c r="K63" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L63" s="14">
         <v>1</v>
       </c>
       <c r="M63" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N63" s="14">
         <v>0</v>
@@ -11596,15 +11666,15 @@
         <v>0</v>
       </c>
       <c r="P63" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q63" s="14" t="s">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="Q63" s="14">
+        <v>1</v>
       </c>
       <c r="R63" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S63" t="s">
+      <c r="S63" s="14" t="s">
         <v>112</v>
       </c>
       <c r="T63" t="s">
@@ -11613,8 +11683,8 @@
       <c r="U63" t="s">
         <v>112</v>
       </c>
-      <c r="V63" s="14" t="s">
-        <v>113</v>
+      <c r="V63" t="s">
+        <v>112</v>
       </c>
       <c r="W63" s="14" t="s">
         <v>113</v>
@@ -11661,8 +11731,8 @@
       <c r="AK63" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AL63" s="14">
-        <v>0</v>
+      <c r="AL63" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AM63" s="14">
         <v>0</v>
@@ -11682,16 +11752,16 @@
         <v>0</v>
       </c>
       <c r="K64" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64" s="17">
         <v>1</v>
       </c>
       <c r="M64" s="17">
-        <v>0</v>
-      </c>
-      <c r="N64" s="17" t="s">
-        <v>112</v>
+        <v>1</v>
+      </c>
+      <c r="N64" s="17">
+        <v>0</v>
       </c>
       <c r="O64" s="17" t="s">
         <v>112</v>
@@ -11705,7 +11775,9 @@
       <c r="R64" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S64" s="17"/>
+      <c r="S64" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="T64" s="17"/>
       <c r="U64" s="17"/>
       <c r="V64" s="17"/>
@@ -11737,15 +11809,17 @@
         <v>0</v>
       </c>
       <c r="K65" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65" s="17">
         <v>1</v>
       </c>
       <c r="M65" s="17">
-        <v>0</v>
-      </c>
-      <c r="N65" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="N65" s="17">
+        <v>0</v>
+      </c>
       <c r="O65" s="17"/>
       <c r="P65" s="17"/>
       <c r="Q65" s="17"/>
@@ -11782,15 +11856,17 @@
         <v>0</v>
       </c>
       <c r="K66" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L66" s="17">
         <v>1</v>
       </c>
       <c r="M66" s="17">
-        <v>0</v>
-      </c>
-      <c r="N66" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="N66" s="17">
+        <v>0</v>
+      </c>
       <c r="O66" s="17"/>
       <c r="P66" s="17"/>
       <c r="Q66" s="17"/>
@@ -11827,15 +11903,17 @@
         <v>0</v>
       </c>
       <c r="K67" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L67" s="20">
         <v>1</v>
       </c>
       <c r="M67" s="20">
-        <v>0</v>
-      </c>
-      <c r="N67" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="N67" s="20">
+        <v>0</v>
+      </c>
       <c r="O67" s="20"/>
       <c r="P67" s="20"/>
       <c r="Q67" s="20"/>
@@ -11872,25 +11950,25 @@
         <v>0</v>
       </c>
       <c r="K68" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L68" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M68" s="11">
         <v>1</v>
       </c>
       <c r="N68" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O68" s="11">
-        <v>0</v>
-      </c>
-      <c r="P68" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q68" s="11" t="s">
-        <v>112</v>
+        <v>1</v>
+      </c>
+      <c r="P68" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="11">
+        <v>0</v>
       </c>
       <c r="R68" s="11" t="s">
         <v>112</v>
@@ -11901,8 +11979,12 @@
       <c r="T68" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="U68" s="11"/>
-      <c r="V68" s="11"/>
+      <c r="U68" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="V68" s="11" t="s">
+        <v>112</v>
+      </c>
       <c r="W68" s="11"/>
       <c r="X68" s="11"/>
       <c r="Y68" s="11"/>
@@ -11931,37 +12013,41 @@
         <v>0</v>
       </c>
       <c r="K69" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L69" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M69" s="17">
         <v>1</v>
       </c>
-      <c r="N69" s="28">
-        <v>0</v>
-      </c>
-      <c r="O69" s="28">
-        <v>0</v>
-      </c>
-      <c r="P69" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q69" s="17" t="s">
-        <v>112</v>
+      <c r="N69" s="17">
+        <v>1</v>
+      </c>
+      <c r="O69" s="17">
+        <v>1</v>
+      </c>
+      <c r="P69" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="28">
+        <v>0</v>
       </c>
       <c r="R69" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S69" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="T69" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="U69" s="17"/>
-      <c r="V69" s="17"/>
+      <c r="S69" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="T69" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="U69" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="V69" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="W69" s="17"/>
       <c r="X69" s="17"/>
       <c r="Y69" s="17"/>
@@ -11990,37 +12076,41 @@
         <v>0</v>
       </c>
       <c r="K70" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L70" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M70" s="14">
         <v>1</v>
       </c>
-      <c r="N70" s="27">
-        <v>0</v>
-      </c>
-      <c r="O70" s="27">
-        <v>1</v>
-      </c>
-      <c r="P70" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q70" s="14" t="s">
-        <v>112</v>
+      <c r="N70" s="14">
+        <v>1</v>
+      </c>
+      <c r="O70" s="14">
+        <v>1</v>
+      </c>
+      <c r="P70" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="27">
+        <v>1</v>
       </c>
       <c r="R70" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S70" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="T70" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="U70" s="14"/>
-      <c r="V70" s="14"/>
+      <c r="S70" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="T70" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="U70" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="V70" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="W70" s="14"/>
       <c r="X70" s="14"/>
       <c r="Y70" s="14"/>
@@ -12049,37 +12139,41 @@
         <v>0</v>
       </c>
       <c r="K71" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M71" s="17">
         <v>1</v>
       </c>
-      <c r="N71" s="28">
-        <v>0</v>
-      </c>
-      <c r="O71" s="28">
-        <v>1</v>
-      </c>
-      <c r="P71" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q71" s="17" t="s">
-        <v>112</v>
+      <c r="N71" s="17">
+        <v>1</v>
+      </c>
+      <c r="O71" s="17">
+        <v>1</v>
+      </c>
+      <c r="P71" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="28">
+        <v>1</v>
       </c>
       <c r="R71" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S71" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="T71" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="U71" s="17"/>
-      <c r="V71" s="17"/>
+      <c r="S71" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="T71" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="U71" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="V71" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="W71" s="17"/>
       <c r="X71" s="17"/>
       <c r="Y71" s="17"/>
@@ -12108,37 +12202,41 @@
         <v>0</v>
       </c>
       <c r="K72" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M72" s="14">
         <v>1</v>
       </c>
-      <c r="N72" s="27">
-        <v>1</v>
-      </c>
-      <c r="O72" s="27">
-        <v>0</v>
-      </c>
-      <c r="P72" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q72" s="14" t="s">
-        <v>112</v>
+      <c r="N72" s="14">
+        <v>1</v>
+      </c>
+      <c r="O72" s="14">
+        <v>1</v>
+      </c>
+      <c r="P72" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="27">
+        <v>0</v>
       </c>
       <c r="R72" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S72" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="T72" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="U72" s="14"/>
-      <c r="V72" s="14"/>
+      <c r="S72" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="T72" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="U72" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="V72" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="W72" s="14"/>
       <c r="X72" s="14"/>
       <c r="Y72" s="14"/>
@@ -12167,37 +12265,41 @@
         <v>0</v>
       </c>
       <c r="K73" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M73" s="17">
         <v>1</v>
       </c>
-      <c r="N73" s="28">
-        <v>1</v>
-      </c>
-      <c r="O73" s="28">
-        <v>0</v>
-      </c>
-      <c r="P73" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q73" s="17" t="s">
-        <v>112</v>
+      <c r="N73" s="17">
+        <v>1</v>
+      </c>
+      <c r="O73" s="17">
+        <v>1</v>
+      </c>
+      <c r="P73" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="28">
+        <v>0</v>
       </c>
       <c r="R73" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S73" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="T73" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="U73" s="17"/>
-      <c r="V73" s="17"/>
+      <c r="S73" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="T73" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="U73" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="V73" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="W73" s="17"/>
       <c r="X73" s="17"/>
       <c r="Y73" s="17"/>
@@ -12226,37 +12328,41 @@
         <v>0</v>
       </c>
       <c r="K74" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74" s="14">
         <v>1</v>
       </c>
-      <c r="N74" s="27">
-        <v>1</v>
-      </c>
-      <c r="O74" s="27">
-        <v>1</v>
-      </c>
-      <c r="P74" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q74" s="14" t="s">
-        <v>112</v>
+      <c r="N74" s="14">
+        <v>1</v>
+      </c>
+      <c r="O74" s="14">
+        <v>1</v>
+      </c>
+      <c r="P74" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="27">
+        <v>1</v>
       </c>
       <c r="R74" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="S74" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="T74" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="U74" s="14"/>
-      <c r="V74" s="14"/>
+      <c r="S74" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="T74" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="U74" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="V74" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="W74" s="14"/>
       <c r="X74" s="14"/>
       <c r="Y74" s="14"/>
@@ -12285,10 +12391,10 @@
         <v>0</v>
       </c>
       <c r="K75" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M75" s="20">
         <v>1</v>
@@ -12299,23 +12405,27 @@
       <c r="O75" s="20">
         <v>1</v>
       </c>
-      <c r="P75" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q75" s="17" t="s">
-        <v>112</v>
+      <c r="P75" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="20">
+        <v>1</v>
       </c>
       <c r="R75" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="S75" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="T75" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="U75" s="20"/>
-      <c r="V75" s="20"/>
+      <c r="S75" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="T75" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="U75" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="V75" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="W75" s="20"/>
       <c r="X75" s="20"/>
       <c r="Y75" s="20"/>
@@ -12340,44 +12450,44 @@
       <c r="I76" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="J76" s="25">
-        <v>1</v>
-      </c>
-      <c r="K76" s="25">
-        <v>0</v>
-      </c>
-      <c r="L76" s="25">
-        <v>0</v>
-      </c>
-      <c r="M76" s="25">
-        <v>0</v>
-      </c>
-      <c r="N76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="O76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="P76" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q76" s="25" t="s">
-        <v>113</v>
+      <c r="J76" s="33">
+        <v>0</v>
+      </c>
+      <c r="K76" s="33">
+        <v>0</v>
+      </c>
+      <c r="L76" s="33">
+        <v>0</v>
+      </c>
+      <c r="M76" s="33">
+        <v>0</v>
+      </c>
+      <c r="N76" s="25">
+        <v>1</v>
+      </c>
+      <c r="O76" s="25">
+        <v>0</v>
+      </c>
+      <c r="P76" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="25">
+        <v>0</v>
       </c>
       <c r="R76" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="S76" s="11">
-        <v>0</v>
-      </c>
-      <c r="T76" s="11">
-        <v>0</v>
-      </c>
-      <c r="U76" s="11">
-        <v>0</v>
-      </c>
-      <c r="V76" s="11">
-        <v>0</v>
+      <c r="S76" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="T76" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="U76" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="V76" s="25" t="s">
+        <v>113</v>
       </c>
       <c r="W76" s="11">
         <v>0</v>
@@ -12441,44 +12551,44 @@
       <c r="I77" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="J77" s="25">
-        <v>1</v>
-      </c>
-      <c r="K77" s="25">
-        <v>0</v>
-      </c>
-      <c r="L77" s="25">
-        <v>0</v>
-      </c>
-      <c r="M77" s="25">
-        <v>1</v>
-      </c>
-      <c r="N77" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="O77" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="P77" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q77" s="25" t="s">
-        <v>113</v>
+      <c r="J77" s="33">
+        <v>0</v>
+      </c>
+      <c r="K77" s="33">
+        <v>0</v>
+      </c>
+      <c r="L77" s="33">
+        <v>0</v>
+      </c>
+      <c r="M77" s="33">
+        <v>0</v>
+      </c>
+      <c r="N77" s="25">
+        <v>1</v>
+      </c>
+      <c r="O77" s="25">
+        <v>0</v>
+      </c>
+      <c r="P77" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="25">
+        <v>1</v>
       </c>
       <c r="R77" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="S77" s="11">
-        <v>0</v>
-      </c>
-      <c r="T77" s="11">
-        <v>0</v>
-      </c>
-      <c r="U77" s="11">
-        <v>0</v>
-      </c>
-      <c r="V77" s="11">
-        <v>0</v>
+      <c r="S77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="T77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="U77" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="V77" s="25" t="s">
+        <v>113</v>
       </c>
       <c r="W77" s="11">
         <v>0</v>
@@ -12542,44 +12652,44 @@
       <c r="I78" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="J78" s="25">
-        <v>1</v>
-      </c>
-      <c r="K78" s="25">
-        <v>0</v>
-      </c>
-      <c r="L78" s="25">
-        <v>1</v>
-      </c>
-      <c r="M78" s="25">
-        <v>0</v>
-      </c>
-      <c r="N78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="O78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="P78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q78" s="25" t="s">
-        <v>112</v>
+      <c r="J78" s="33">
+        <v>0</v>
+      </c>
+      <c r="K78" s="33">
+        <v>0</v>
+      </c>
+      <c r="L78" s="33">
+        <v>0</v>
+      </c>
+      <c r="M78" s="33">
+        <v>0</v>
+      </c>
+      <c r="N78" s="25">
+        <v>1</v>
+      </c>
+      <c r="O78" s="25">
+        <v>0</v>
+      </c>
+      <c r="P78" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="25">
+        <v>0</v>
       </c>
       <c r="R78" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="S78" s="25">
-        <v>0</v>
-      </c>
-      <c r="T78" s="25">
-        <v>0</v>
-      </c>
-      <c r="U78" s="25">
-        <v>0</v>
-      </c>
-      <c r="V78" s="25">
-        <v>0</v>
+      <c r="S78" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="T78" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="U78" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="V78" s="25" t="s">
+        <v>112</v>
       </c>
       <c r="W78" s="25">
         <v>0</v>
@@ -12643,7 +12753,6 @@
   <mergeCells count="15">
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="J1:M1"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
@@ -12656,6 +12765,7 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>